<commit_message>
ver 25.04 con HMI 3.2 10/02/2025
Macchina fiera in India + macchina Pimkie con firmware m32_0004_V2_10_x18_01_c2.bin, risolve problema spostamento XY + motori XY meno vibrazioni
</commit_message>
<xml_diff>
--- a/IO_varie_versioni.xlsx
+++ b/IO_varie_versioni.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="352">
   <si>
     <t>//******************************************************************</t>
   </si>
@@ -694,6 +694,384 @@
   </si>
   <si>
     <t>o59_CarPat_SoffioPattina</t>
+  </si>
+  <si>
+    <t>882 inclinata</t>
+  </si>
+  <si>
+    <t>o18_C1_bloccaFiloMagente</t>
+  </si>
+  <si>
+    <t>o2</t>
+  </si>
+  <si>
+    <t>o1_Enable_AssiXY_C1C2</t>
+  </si>
+  <si>
+    <t>o3_C1_Pinza_int</t>
+  </si>
+  <si>
+    <t>o4_C1_Pinza_est</t>
+  </si>
+  <si>
+    <t>o5_C1_Ranocchia_retrat</t>
+  </si>
+  <si>
+    <t>o6_Pinza_carico_Su_Giu</t>
+  </si>
+  <si>
+    <t>o7_C1_Cambio_Pinze</t>
+  </si>
+  <si>
+    <t>o8_C1_Retrattile_AC</t>
+  </si>
+  <si>
+    <t>o9_C1_rasafilo</t>
+  </si>
+  <si>
+    <t>o10_Lancia_AD</t>
+  </si>
+  <si>
+    <t>o11_Lentezza_Tasca_AD</t>
+  </si>
+  <si>
+    <t>o12_Cambio_Lamelle_4_5</t>
+  </si>
+  <si>
+    <t>o13_C1_Piedino</t>
+  </si>
+  <si>
+    <t>o14_C1_Scalino_Piedino</t>
+  </si>
+  <si>
+    <t>o15_C1_RaffreddamentoAgo</t>
+  </si>
+  <si>
+    <t>o16_Piegatore_AD</t>
+  </si>
+  <si>
+    <t>o17_Piegatore_Su_Giu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> o19_Bilanciere_Su_Giu</t>
+  </si>
+  <si>
+    <t>o20_Piegatore_4</t>
+  </si>
+  <si>
+    <t>o21_Piegatore_1</t>
+  </si>
+  <si>
+    <t>o22_Piegatore_2</t>
+  </si>
+  <si>
+    <t>o23_Piegatore_3</t>
+  </si>
+  <si>
+    <t>o24_Cambio_lame_lateral</t>
+  </si>
+  <si>
+    <t>o25_Cambio_lama_front</t>
+  </si>
+  <si>
+    <t>o26_Cambio_corpo</t>
+  </si>
+  <si>
+    <t>o27_EvAspiratore</t>
+  </si>
+  <si>
+    <t>o28_Valvolone</t>
+  </si>
+  <si>
+    <t>o31</t>
+  </si>
+  <si>
+    <t>o32</t>
+  </si>
+  <si>
+    <t>o34</t>
+  </si>
+  <si>
+    <t>o36</t>
+  </si>
+  <si>
+    <t>o37</t>
+  </si>
+  <si>
+    <t>o38</t>
+  </si>
+  <si>
+    <t>o41_C2_rasafilo</t>
+  </si>
+  <si>
+    <t>o42</t>
+  </si>
+  <si>
+    <t>o43_C2_RaffreddamentoAgo</t>
+  </si>
+  <si>
+    <t>o45_C2_Piedino</t>
+  </si>
+  <si>
+    <t>o46</t>
+  </si>
+  <si>
+    <t>o48_Prima_barra</t>
+  </si>
+  <si>
+    <t>o50</t>
+  </si>
+  <si>
+    <t>o51</t>
+  </si>
+  <si>
+    <t>o52</t>
+  </si>
+  <si>
+    <t>o53_C2_Scalino_Piedino</t>
+  </si>
+  <si>
+    <t>o54_C2_bloccaFiloMagente</t>
+  </si>
+  <si>
+    <t>o56</t>
+  </si>
+  <si>
+    <t>o57</t>
+  </si>
+  <si>
+    <t>o58</t>
+  </si>
+  <si>
+    <t>o59</t>
+  </si>
+  <si>
+    <t>o62_Pinza_tras_su_giu</t>
+  </si>
+  <si>
+    <t>o64_Scaric_dx_sx</t>
+  </si>
+  <si>
+    <t>i4_Pressostato</t>
+  </si>
+  <si>
+    <t>i5_Emg</t>
+  </si>
+  <si>
+    <t>i6_ROtturaFilo</t>
+  </si>
+  <si>
+    <t>i7_C1_FcMinAsseX</t>
+  </si>
+  <si>
+    <t>i8_C1_FcMaxAsseY</t>
+  </si>
+  <si>
+    <t>i9_C1_FcMinAsseY</t>
+  </si>
+  <si>
+    <t>i10</t>
+  </si>
+  <si>
+    <t>i11_C1_FcZeroAgo</t>
+  </si>
+  <si>
+    <t>i12_FcPinzaCaricoAlta</t>
+  </si>
+  <si>
+    <t>i13_C1_PinzaIntBassa</t>
+  </si>
+  <si>
+    <t>i14_C1_PinzaEstAlta</t>
+  </si>
+  <si>
+    <t>i15_C1_FcZeroCrochet</t>
+  </si>
+  <si>
+    <t>i16_FcPiegatore_AV</t>
+  </si>
+  <si>
+    <t>i17_FcPiegatore_DI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i18_FcMinCaricatore1 </t>
+  </si>
+  <si>
+    <t>i19_FcPiegatoreBasso</t>
+  </si>
+  <si>
+    <t>i20_FcLancia_DI</t>
+  </si>
+  <si>
+    <t>i21_PulsResetFolder</t>
+  </si>
+  <si>
+    <t>i22_C1_PulsStopTesta</t>
+  </si>
+  <si>
+    <t>i23_Rinforzo_ready</t>
+  </si>
+  <si>
+    <t>i24                     din24</t>
+  </si>
+  <si>
+    <t>i25_Rinforzo_Attivo</t>
+  </si>
+  <si>
+    <t>i26_C1_ReadyAsseX</t>
+  </si>
+  <si>
+    <t>i27                     din27</t>
+  </si>
+  <si>
+    <t>i28                     din28</t>
+  </si>
+  <si>
+    <t>i29                     din29</t>
+  </si>
+  <si>
+    <t>i30_C1_ReadyAsseY</t>
+  </si>
+  <si>
+    <t>i34_C2_Pedana</t>
+  </si>
+  <si>
+    <t>i38_C2_RotturaFilo</t>
+  </si>
+  <si>
+    <t>i39_C2_FcMinAsseX</t>
+  </si>
+  <si>
+    <t>i40_C2_FcMaxAsseY</t>
+  </si>
+  <si>
+    <t>i41_C2_FcMinAsseY</t>
+  </si>
+  <si>
+    <t>i42</t>
+  </si>
+  <si>
+    <t>i44</t>
+  </si>
+  <si>
+    <t>i45_C2_FcPinzaIntBassa</t>
+  </si>
+  <si>
+    <t>i46</t>
+  </si>
+  <si>
+    <t>i47_C2_FcZeroCrochet</t>
+  </si>
+  <si>
+    <t>i48</t>
+  </si>
+  <si>
+    <t>i49_FcPinzaTraslAlta</t>
+  </si>
+  <si>
+    <t>i51</t>
+  </si>
+  <si>
+    <t>i52</t>
+  </si>
+  <si>
+    <t>i53</t>
+  </si>
+  <si>
+    <t>i54_C2_PulsStopTesta</t>
+  </si>
+  <si>
+    <t>i55</t>
+  </si>
+  <si>
+    <t>i58_C2_ReadyAsseX</t>
+  </si>
+  <si>
+    <t>i62_C2_ReadyAsseY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i31_Bilanciere_Alto     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i32_Bilanciere_Basso   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i33                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i35                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i36                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i37                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">882 inclinata </t>
+  </si>
+  <si>
+    <t>out come Argentina</t>
+  </si>
+  <si>
+    <t>irq</t>
+  </si>
+  <si>
+    <t>non collegare</t>
+  </si>
+  <si>
+    <t>i43_C2_FcZeroAgo</t>
+  </si>
+  <si>
+    <t>i50_FcMinCaricatore2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>o33_Enable_AssiXY_C2</t>
+  </si>
+  <si>
+    <t>o49_Seconda_barra</t>
+  </si>
+  <si>
+    <t>inclinata out come Argentina</t>
+  </si>
+  <si>
+    <t>NON E' PIU' COSI'</t>
+  </si>
+  <si>
+    <t>ORA E' COSI'</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_Top_SUGIu := i41;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_Middle_SUGIu := i42;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_Bottom_SUGIu := i43;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_Tastatore := i44;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_Empty := i45;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_BackPos :=i46;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vb_ingresso_CarPat_SpoLamLungoL :=i61;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_SpoLamLungoR :=i62;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_SpoLamCortoL :=i63;</t>
+  </si>
+  <si>
+    <t>Vb_ingresso_CarPat_SpoLamCortoR :=i64;</t>
   </si>
 </sst>
 </file>
@@ -717,7 +1095,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,6 +1120,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -755,12 +1139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1062,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M143"/>
+  <dimension ref="B1:Q165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,320 +1458,528 @@
     <col min="2" max="2" width="32.140625" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>77</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>78</v>
       </c>
       <c r="L7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="L8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>79</v>
       </c>
       <c r="L10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>80</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>81</v>
       </c>
       <c r="L12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>82</v>
       </c>
       <c r="L13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="L14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="L15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="L16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="L17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="L18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>84</v>
       </c>
       <c r="L19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="L20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>85</v>
       </c>
       <c r="L21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>86</v>
       </c>
       <c r="L22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>87</v>
       </c>
       <c r="L23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>88</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>89</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>90</v>
       </c>
       <c r="L26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>91</v>
       </c>
       <c r="L28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>92</v>
       </c>
       <c r="L29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>93</v>
       </c>
       <c r="L30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>94</v>
       </c>
       <c r="L31" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q31">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>95</v>
       </c>
       <c r="L32" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>96</v>
       </c>
       <c r="L33" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>97</v>
       </c>
       <c r="L34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>98</v>
       </c>
       <c r="L35" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>99</v>
       </c>
       <c r="L36" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>100</v>
       </c>
       <c r="L37" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>101</v>
       </c>
       <c r="L38" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>102</v>
       </c>
       <c r="L39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q39">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>103</v>
       </c>
       <c r="L40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>104</v>
       </c>
       <c r="L41" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P41" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>105</v>
       </c>
@@ -1396,16 +1989,25 @@
       <c r="L42" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>106</v>
       </c>
       <c r="L43" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>107</v>
       </c>
@@ -1415,96 +2017,156 @@
       <c r="L44" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q44">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>108</v>
       </c>
       <c r="L45" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P45" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>109</v>
       </c>
       <c r="L46" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P46" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q46">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>110</v>
       </c>
       <c r="L47" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>4</v>
       </c>
       <c r="L48" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P48" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q48">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>111</v>
       </c>
       <c r="L49" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P49" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>112</v>
       </c>
       <c r="L50" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P50" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q50">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>113</v>
       </c>
       <c r="L51" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P51" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>114</v>
       </c>
       <c r="L52" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P52" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q52">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>115</v>
       </c>
       <c r="L53" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P53" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>116</v>
       </c>
       <c r="L54" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P54" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q54">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>5</v>
       </c>
       <c r="L55" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P55" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q55">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>117</v>
       </c>
@@ -1514,8 +2176,14 @@
       <c r="L56" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P56" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>118</v>
       </c>
@@ -1525,16 +2193,22 @@
       <c r="L57" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>119</v>
       </c>
       <c r="L58" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P58" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>120</v>
       </c>
@@ -1544,626 +2218,1086 @@
       <c r="L59" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P59" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>121</v>
       </c>
       <c r="L60" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P60" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>122</v>
       </c>
       <c r="L61" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>123</v>
       </c>
       <c r="L62" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>124</v>
       </c>
       <c r="L63" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P63" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q63">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>125</v>
       </c>
       <c r="L64" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>126</v>
       </c>
       <c r="L65" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>127</v>
       </c>
       <c r="L66" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>128</v>
       </c>
       <c r="L67" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P67" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q67">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>129</v>
       </c>
       <c r="L68" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>130</v>
       </c>
       <c r="L69" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="P69" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q71" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q72" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q73" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q74" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q75" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q76" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q79" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q80" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q81" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q82" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P88" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q88" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L79" s="1" t="s">
+      <c r="L89" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B80" s="3" t="s">
+      <c r="P89" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q89" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B90" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L80" s="3" t="s">
+      <c r="L90" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
+      <c r="P90" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q90">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B91" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L81" s="3" t="s">
+      <c r="L91" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
+      <c r="P91" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B92" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L82" s="3" t="s">
+      <c r="L92" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B83" s="3" t="s">
+      <c r="P92" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q92">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L83" s="3" t="s">
+      <c r="L93" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
+      <c r="P93" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q93">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="L84" s="3" t="s">
+      <c r="L94" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B85" s="3" t="s">
+      <c r="P94" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q94">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B95" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L85" s="3" t="s">
+      <c r="L95" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B86" s="3" t="s">
+      <c r="P95" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q95">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B96" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="L86" s="3" t="s">
+      <c r="L96" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B87" s="3" t="s">
+      <c r="P96" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q96">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B97" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="L87" s="3" t="s">
+      <c r="L97" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
+      <c r="P97" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q97">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B98" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="L88" s="3" t="s">
+      <c r="L98" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B89" s="3" t="s">
+      <c r="P98" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q98">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L89" s="3" t="s">
+      <c r="L99" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B90" s="3" t="s">
+      <c r="P99" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B100" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="L90" s="3" t="s">
+      <c r="L100" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
+      <c r="P100" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q100">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B101" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L91" s="3" t="s">
+      <c r="L101" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
+      <c r="P101" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B102" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="L92" s="3" t="s">
+      <c r="L102" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B93" s="3" t="s">
+      <c r="P102" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q102">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B103" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="L93" s="3" t="s">
+      <c r="L103" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B94" s="3" t="s">
+      <c r="P103" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q103">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B104" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L94" s="3" t="s">
+      <c r="L104" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
+      <c r="P104" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q104">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="L95" s="3" t="s">
+      <c r="L105" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B96" s="3" t="s">
+      <c r="P105" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q105">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="L96" s="3" t="s">
+      <c r="L106" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B97" s="3" t="s">
+      <c r="P106" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q106">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B107" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L97" s="3" t="s">
+      <c r="L107" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B98" s="3" t="s">
+      <c r="P107" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q107">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B108" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="L98" s="3" t="s">
+      <c r="L108" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B99" s="3" t="s">
+      <c r="P108" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q108">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B109" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L99" s="3" t="s">
+      <c r="L109" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B100" s="3" t="s">
+      <c r="P109" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B110" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="L100" s="3" t="s">
+      <c r="L110" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B101" s="3" t="s">
+      <c r="P110" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B111" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="L101" s="3" t="s">
+      <c r="L111" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B102" s="3" t="s">
+      <c r="P111" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B112" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L102" s="3" t="s">
+      <c r="L112" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B103" s="3" t="s">
+      <c r="P112" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B113" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L103" s="3" t="s">
+      <c r="L113" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B104" s="3" t="s">
+      <c r="P113" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q113">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B114" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L104" s="3" t="s">
+      <c r="L114" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B105" s="3" t="s">
+      <c r="P114" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B115" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="L105" s="3" t="s">
+      <c r="L115" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B106" s="3" t="s">
+      <c r="P115" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q115">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B116" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="L106" s="3" t="s">
+      <c r="L116" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+      <c r="P116" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q116">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>192</v>
       </c>
-      <c r="L107" s="4" t="s">
+      <c r="L117" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+      <c r="P117" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q117">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
         <v>193</v>
       </c>
-      <c r="L108" s="4" t="s">
+      <c r="L118" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+      <c r="P118" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="119" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
         <v>194</v>
       </c>
-      <c r="L109" s="4" t="s">
+      <c r="L119" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B110" s="3" t="s">
+      <c r="P119" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="120" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B120" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="L110" s="3" t="s">
+      <c r="L120" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B111" s="3" t="s">
+      <c r="P120" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B121" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="L111" s="3" t="s">
+      <c r="L121" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B112" s="3" t="s">
+      <c r="P121" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="122" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B122" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="L112" s="3" t="s">
+      <c r="L122" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B113" s="2" t="s">
+      <c r="P122" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q122">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L113" s="2" t="s">
+      <c r="L123" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B114" s="2" t="s">
+      <c r="P123" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="124" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B124" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="L114" s="2" t="s">
+      <c r="L124" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B115" s="2" t="s">
+      <c r="P124" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q124">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B125" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="L115" s="2" t="s">
+      <c r="L125" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B116" s="2" t="s">
+      <c r="P125" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B126" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L116" s="2" t="s">
+      <c r="L126" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B117" s="2" t="s">
+      <c r="P126" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B127" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="L117" s="2" t="s">
+      <c r="L127" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B118" s="2" t="s">
+      <c r="P127" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B128" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="L118" s="2" t="s">
+      <c r="L128" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
+      <c r="P128" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q128">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
         <v>201</v>
       </c>
-      <c r="L119" s="2" t="s">
+      <c r="L129" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B120" s="2" t="s">
+      <c r="P129" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B130" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="L120" s="2" t="s">
+      <c r="L130" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="M120" t="s">
+      <c r="M130" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B121" s="2" t="s">
+      <c r="P130" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q130">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B131" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="L121" s="2" t="s">
+      <c r="L131" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B122" s="2" t="s">
+      <c r="P131" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B132" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="L122" s="2" t="s">
+      <c r="L132" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
+      <c r="P132" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q132">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
         <v>177</v>
       </c>
-      <c r="L123" t="s">
+      <c r="L133" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
+      <c r="P133" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
         <v>178</v>
       </c>
-      <c r="L124" t="s">
+      <c r="L134" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B125" s="3" t="s">
+      <c r="P134" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q134">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="L125" s="3" t="s">
+      <c r="L135" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
+      <c r="P135" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
         <v>203</v>
       </c>
-      <c r="L126" s="2" t="s">
+      <c r="L136" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B127" s="3" t="s">
+      <c r="P136" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B137" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="L127" s="3" t="s">
+      <c r="L137" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B128" s="2" t="s">
+      <c r="P137" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q137">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B138" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L128" s="2" t="s">
+      <c r="L138" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B129" s="2" t="s">
+      <c r="P138" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q138">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B139" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="L129" s="2" t="s">
+      <c r="L139" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B130" s="3" t="s">
+      <c r="P139" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B140" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L130" s="3" t="s">
+      <c r="L140" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B131" s="3" t="s">
+      <c r="P140" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B141" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L131" s="3" t="s">
+      <c r="L141" s="3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B132" s="2" t="s">
+      <c r="P141" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B142" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="L132" s="2" t="s">
+      <c r="L142" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B133" s="2" t="s">
+      <c r="P142" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q142">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B143" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="L133" s="2" t="s">
+      <c r="L143" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
+      <c r="P143" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q143">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
         <v>210</v>
       </c>
-      <c r="L134" s="2" t="s">
+      <c r="L144" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B135" s="2" t="s">
+      <c r="P144" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B145" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="L135" s="2" t="s">
+      <c r="L145" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B136" s="2" t="s">
+      <c r="P145" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B146" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="L136" s="2" t="s">
+      <c r="L146" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B137" s="2" t="s">
+      <c r="P146" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B147" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="L137" s="2" t="s">
+      <c r="L147" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B138" s="2" t="s">
+      <c r="P147" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B148" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C148" t="s">
         <v>218</v>
       </c>
-      <c r="L138" s="2" t="s">
+      <c r="L148" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B139" s="2" t="s">
+      <c r="P148" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B149" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="L139" t="s">
+      <c r="L149" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B140" s="2" t="s">
+      <c r="P149" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B150" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="L140" t="s">
+      <c r="L150" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
+      <c r="P150" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
         <v>188</v>
       </c>
-      <c r="L141" t="s">
+      <c r="L151" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B142" s="2" t="s">
+      <c r="P151" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q151">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B152" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="L142" t="s">
+      <c r="L152" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
+      <c r="P152" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
         <v>190</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L153" t="s">
         <v>190</v>
+      </c>
+      <c r="P153" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q153">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q157" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q158" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q159" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q160" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="161" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q161" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="162" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q162" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="163" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q163" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="164" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q164" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="165" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q165" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>